<commit_message>
Added more documentation to README.md regarding Labeller.py
Modified Name_Attacher.py to make it so that the function takes and returns a DataFrame.
File handling will be handled by main function.

Modified the Labeller.py in a similar fashion.
</commit_message>
<xml_diff>
--- a/Timetable/new_mal_1.xlsx
+++ b/Timetable/new_mal_1.xlsx
@@ -539,8 +539,14 @@
           <t>3 4</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
     </row>
@@ -575,8 +581,14 @@
           <t>6 7</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
     </row>
@@ -611,8 +623,14 @@
           <t>8 9</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
     </row>
@@ -647,8 +665,14 @@
           <t>1 2</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
     </row>
@@ -683,8 +707,14 @@
           <t>3 4</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
     </row>
@@ -719,8 +749,14 @@
           <t>6 7</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
     </row>
@@ -755,8 +791,14 @@
           <t>8 9</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>1</v>
+      </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
     </row>
@@ -791,8 +833,14 @@
           <t>1 2</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
     </row>
@@ -827,8 +875,14 @@
           <t>3 4</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
     </row>
@@ -863,8 +917,14 @@
           <t>6 7</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
     </row>
@@ -899,8 +959,14 @@
           <t>8 9</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
     </row>
@@ -935,8 +1001,14 @@
           <t>1 2</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
     </row>
@@ -971,8 +1043,14 @@
           <t>3 4</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
+      </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
     </row>
@@ -1007,8 +1085,14 @@
           <t>6 7</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>1</v>
+      </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
     </row>
@@ -1043,8 +1127,14 @@
           <t>8 9</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
     </row>
@@ -1079,8 +1169,14 @@
           <t>1 2</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
     </row>
@@ -1115,8 +1211,14 @@
           <t>3 4</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
     </row>
@@ -1151,8 +1253,14 @@
           <t>6 7</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
     </row>
@@ -1187,8 +1295,14 @@
           <t>8 9</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
     </row>
@@ -1223,8 +1337,14 @@
           <t>1 2</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
     </row>
@@ -1259,8 +1379,14 @@
           <t>3 4</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Just an update after a long time. Not sure what has changed, but commiting it for now.
</commit_message>
<xml_diff>
--- a/Timetable/new_mal_1.xlsx
+++ b/Timetable/new_mal_1.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -42883,6 +42883,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>